<commit_message>
Update 1.8.4: Invoice Return Bug fixes
</commit_message>
<xml_diff>
--- a/pkg/excels/templates/Invoice Return Report.xlsx
+++ b/pkg/excels/templates/Invoice Return Report.xlsx
@@ -1,22 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mamad\OneDrive\Desktop\ТГЭМ\backend-v2\pkg\excels\report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Desktop\TGEM\tgem-backend\pkg\excels\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A4053F-D865-443A-ACF4-CB7D46DB559C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -55,15 +53,23 @@
     <t>Цена</t>
   </si>
   <si>
-    <t>Из них негодно</t>
+    <t>Брак</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -80,12 +86,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -93,16 +99,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -379,57 +403,60 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.21875" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" customWidth="1"/>
-    <col min="4" max="5" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="7" max="7" width="11.77734375" customWidth="1"/>
-    <col min="8" max="8" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="J1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>